<commit_message>
updated iceburg chart to  be color coded to classes
</commit_message>
<xml_diff>
--- a/iceburgchart.xlsx
+++ b/iceburgchart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dane.hixson\Desktop\cs 2450_project_part2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dane.hixson\Documents\cs_2450_group_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
   <si>
     <t>Priority</t>
   </si>
@@ -99,9 +99,6 @@
     <t>On startup, the program reads from the Books file</t>
   </si>
   <si>
-    <t>Allow user to select the filename</t>
-  </si>
-  <si>
     <t>When program exits, write data back out to the file</t>
   </si>
   <si>
@@ -189,14 +186,26 @@
     <t>Interface: quit</t>
   </si>
   <si>
-    <t>Must allow use date to advance</t>
+    <t>Allow user to select the filename for books</t>
+  </si>
+  <si>
+    <t>Patrons</t>
+  </si>
+  <si>
+    <t>Books/media</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>Interface</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,8 +213,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +248,21 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -228,10 +273,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -246,8 +294,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -264,8 +318,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B34" totalsRowShown="0">
-  <autoFilter ref="A1:B34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B33" totalsRowShown="0">
+  <autoFilter ref="A1:B33"/>
   <sortState ref="A2:B34">
     <sortCondition ref="B1:B34"/>
   </sortState>
@@ -709,19 +763,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="81.44140625" customWidth="1"/>
     <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -729,7 +784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -737,113 +792,125 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F4" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6">
+      <c r="F5" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7">
+      <c r="F6" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>31</v>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>32</v>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="B12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>35</v>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="B13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>36</v>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>37</v>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="B15">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -851,46 +918,46 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>42</v>
+      <c r="A18" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="B18">
         <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>43</v>
+      <c r="A19" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="B19">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>44</v>
+      <c r="A20" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="B20">
         <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>54</v>
+      <c r="A21" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="B21">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B22">
@@ -898,15 +965,15 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B23">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B24">
@@ -914,7 +981,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B25">
@@ -922,7 +989,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" s="8" t="s">
         <v>49</v>
       </c>
       <c r="B26">
@@ -930,7 +997,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="8" t="s">
         <v>50</v>
       </c>
       <c r="B27">
@@ -938,7 +1005,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="8" t="s">
         <v>51</v>
       </c>
       <c r="B28">
@@ -946,7 +1013,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="8" t="s">
         <v>52</v>
       </c>
       <c r="B29">
@@ -954,24 +1021,24 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>53</v>
+      <c r="A30" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="B30">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31">
-        <v>9</v>
+      <c r="A31" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B32" s="5">
         <v>10</v>
@@ -979,17 +1046,9 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B33" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34" s="5">
         <v>10</v>
       </c>
     </row>

</xml_diff>